<commit_message>
Sottomissione TARASOFT 45801 v2.0: aggiornamento
</commit_message>
<xml_diff>
--- a/GATEWAY/tarasoft/tarasoft_/45801/2.0/report-checklist.xlsx
+++ b/GATEWAY/tarasoft/tarasoft_/45801/2.0/report-checklist.xlsx
@@ -1436,123 +1436,63 @@
     <t>bf45ac519b7edf50086ba8e235adcbd7</t>
   </si>
   <si>
-    <t>07.28.00</t>
-  </si>
-  <si>
-    <t>17.01.00</t>
-  </si>
-  <si>
-    <t>18.54.00</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT08_KO</t>
   </si>
   <si>
     <t>ff5893859fee1ff1d9add993ffd99a08</t>
   </si>
   <si>
-    <t>07.54.00</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT09_KO</t>
   </si>
   <si>
-    <t>08.03.00</t>
-  </si>
-  <si>
     <t>6b97fb52545271717e74d3fa33dc5b2b</t>
   </si>
   <si>
-    <t>08.12.00</t>
-  </si>
-  <si>
     <t>1b0dfb9feecd9d1f6d05619780fdebb4</t>
   </si>
   <si>
-    <t>08.25.00</t>
-  </si>
-  <si>
     <t>238366544401a5af2f68a2924b72abb5</t>
   </si>
   <si>
-    <t>08.33.00</t>
-  </si>
-  <si>
     <t>2980f228441067222227d755cbf34877</t>
   </si>
   <si>
-    <t>08.39.00</t>
-  </si>
-  <si>
     <t>847a9f827cba82574887d87fd6ee3181</t>
   </si>
   <si>
-    <t>08.55.00</t>
-  </si>
-  <si>
     <t>c3a4b129aab8ecb19e18bc91caeb79b1</t>
   </si>
   <si>
-    <t>09.03.00</t>
-  </si>
-  <si>
     <t>cc08bf4b5b609cd6343ddf1fafdbe584</t>
   </si>
   <si>
-    <t>10.28.00</t>
-  </si>
-  <si>
     <t>582cfe372aaaba52a1d798a0ac601d2c</t>
   </si>
   <si>
-    <t>10.34.00</t>
-  </si>
-  <si>
     <t>8fe29cc3ec7e1f9ea69f4f55db36f7ef</t>
   </si>
   <si>
-    <t>10.39.00</t>
-  </si>
-  <si>
     <t>fed47ddcb943c6c14eba4b5624ce893c</t>
   </si>
   <si>
-    <t>10.47.00</t>
-  </si>
-  <si>
     <t>9c2c30dfe92ab64b131b003091e243fa</t>
   </si>
   <si>
-    <t>10.54.00</t>
-  </si>
-  <si>
     <t>4243077c7f2e640a36550f7838b03cd4</t>
   </si>
   <si>
-    <t>10.59.00</t>
-  </si>
-  <si>
     <t>ad29d3d46849277f7e7bc88816a310a5</t>
   </si>
   <si>
-    <t>11.04.00</t>
-  </si>
-  <si>
     <t>ddeb775ab5fb0e6ba2265fe5ce7b7021</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT27_KO</t>
   </si>
   <si>
-    <t>11.09.00</t>
-  </si>
-  <si>
     <t>ec8c474898bf854de2f2b718991fea3f</t>
   </si>
   <si>
-    <t>11.14.00</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT28_KO</t>
   </si>
   <si>
@@ -1562,9 +1502,6 @@
     <t>VALIDAZIONE_CDA2_RAD_CT25_OK</t>
   </si>
   <si>
-    <t>16.14.00</t>
-  </si>
-  <si>
     <t>9a56d9d564da1168781347d26c091dc5</t>
   </si>
   <si>
@@ -1574,120 +1511,63 @@
     <t>VALIDAZIONE_CDA2_RAD_CT26_OK</t>
   </si>
   <si>
-    <t>17.09.00</t>
-  </si>
-  <si>
     <t>3383d2f8fa6a422d67eaad9314253f10</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.30.4.4.c22af8628943b0adb82544199d15d420c6cd8e41f8aafdecbf0c09ead259b9a3.c7e3643747^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>05.56.00</t>
-  </si>
-  <si>
     <t>d5752852c2256166990db7f2300e0802</t>
   </si>
   <si>
-    <t>06.02.00</t>
-  </si>
-  <si>
     <t>2e5fe0a8a5dd0ccc0cbe676ea46fc6be</t>
   </si>
   <si>
-    <t>06.07.00</t>
-  </si>
-  <si>
     <t>62e77ae86bb600d57c68b3d0242743c9</t>
   </si>
   <si>
-    <t>06.12.00</t>
-  </si>
-  <si>
     <t>9e4533243aca85b5c482f8caca650c50</t>
   </si>
   <si>
-    <t>06.21.00</t>
-  </si>
-  <si>
     <t>575b07491762f0358e061ba738415070</t>
   </si>
   <si>
-    <t>06.29.00</t>
-  </si>
-  <si>
     <t>044b9ebd672cef670684353a0e58737e</t>
   </si>
   <si>
-    <t>06.35.00</t>
-  </si>
-  <si>
     <t>ca285b08f2cb0e73a3ed1062db4bcb6b</t>
   </si>
   <si>
-    <t>06.40.00</t>
-  </si>
-  <si>
     <t>b2f7b90077fdd78b46524e868149f832</t>
   </si>
   <si>
-    <t>06.46.00</t>
-  </si>
-  <si>
     <t>5541890fc29641380380878a89921dc1</t>
   </si>
   <si>
-    <t>06.50.00</t>
-  </si>
-  <si>
     <t>fbb71cd12c852d3f596c15bc557051c0</t>
   </si>
   <si>
-    <t>07.00.00</t>
-  </si>
-  <si>
     <t>4053f3a389432c418b05be2fb5e7e303</t>
   </si>
   <si>
-    <t>07.05.00</t>
-  </si>
-  <si>
     <t>74bf1964b244be0af2753fc5b4315c2e</t>
   </si>
   <si>
-    <t>07.10.00</t>
-  </si>
-  <si>
     <t>c1e1143094c73df32a9a336f369b0891</t>
   </si>
   <si>
-    <t>07.16.00</t>
-  </si>
-  <si>
     <t>4cb3162e4e6c8c8489e72c4b320a403c</t>
   </si>
   <si>
-    <t>07.22.00</t>
-  </si>
-  <si>
     <t>815620bdbf9e26999ad7e1a461fc5050</t>
   </si>
   <si>
-    <t>07.30.00</t>
-  </si>
-  <si>
     <t>5b7a5aad9ff65603786a49db2d916851</t>
   </si>
   <si>
-    <t>07.34.00</t>
-  </si>
-  <si>
     <t>4d09839b11a460642b547bd68e11a9e2</t>
   </si>
   <si>
-    <t>07.38.00</t>
-  </si>
-  <si>
     <t>90b18d2a0f6ddef1c545137c611cc1f2</t>
   </si>
   <si>
@@ -1763,21 +1643,12 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>10.00.00</t>
-  </si>
-  <si>
-    <t>10.05.00</t>
-  </si>
-  <si>
     <t>31,39,47,76,78,79,80,81,83,84,85,86,87,88,89,90,91,92,93,462,474</t>
   </si>
   <si>
     <t>32,40,48,152,154,155,156,159,160,161,162,163,164,165,166,167,168,169,461,468,475</t>
   </si>
   <si>
-    <t>09.18.00</t>
-  </si>
-  <si>
     <t>b0a671d964e6ce428906b636feb3c55a</t>
   </si>
   <si>
@@ -1787,9 +1658,6 @@
     <t>5753e48983833947e7689639090336e0</t>
   </si>
   <si>
-    <t>09.51.00</t>
-  </si>
-  <si>
     <t>5d0d1e438fd8d44b5252d8bcf01ca926</t>
   </si>
   <si>
@@ -1905,6 +1773,138 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.30.4.4.910128636be06d441b232825151baa3731af884810e3dfd1cb6f9f5893fe1f42.89636a2fe9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-09T08:18:25Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T15:14:21Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T16:09:06Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T04:56:38Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:02:14Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:07:52Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:12:31Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:21:02Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:29:27Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:35:40Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:40:08Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:46:03Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T05:50:16Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:00:54Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:05:54Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:10:46Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:16:05Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:22:16Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:30:18Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:34:02Z</t>
+  </si>
+  <si>
+    <t>2025-12-28T06:38:57Z</t>
+  </si>
+  <si>
+    <t>2026-01-09T08:51:28Z</t>
+  </si>
+  <si>
+    <t>2026-01-08T10:26:05Z</t>
+  </si>
+  <si>
+    <t>2026-01-08T10:05:31Z</t>
+  </si>
+  <si>
+    <t>2025-12-26T16:01:45Z</t>
+  </si>
+  <si>
+    <t>2025-12-26T17:54:42Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T06:28:33Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T06:54:21Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T07:03:41Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T07:12:04Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T07:25:25Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T07:33:11Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T07:39:30Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T07:55:56Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T08:03:31Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T09:28:40Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T09:34:09Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T09:39:14Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T09:47:28Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T09:54:34Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T09:59:58Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T10:04:35Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T10:09:52Z</t>
+  </si>
+  <si>
+    <t>2025-12-27T10:14:39Z</t>
   </si>
 </sst>
 </file>
@@ -4001,10 +4001,10 @@
   <dimension ref="A1:W731"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B170" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S193" sqref="S193"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4013,7 +4013,7 @@
     <col min="2" max="2" width="27.1796875" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" customWidth="1"/>
     <col min="4" max="4" width="40.26953125" customWidth="1"/>
-    <col min="5" max="5" width="104.81640625" customWidth="1"/>
+    <col min="5" max="5" width="46.54296875" customWidth="1"/>
     <col min="6" max="7" width="33.1796875" customWidth="1"/>
     <col min="8" max="8" width="38.26953125" customWidth="1"/>
     <col min="9" max="9" width="143.36328125" bestFit="1" customWidth="1"/>
@@ -9314,7 +9314,7 @@
         <v>38</v>
       </c>
       <c r="D145" s="33" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="E145" s="41" t="s">
         <v>43</v>
@@ -9326,10 +9326,10 @@
         <v>472</v>
       </c>
       <c r="H145" s="35" t="s">
-        <v>473</v>
+        <v>430</v>
       </c>
       <c r="I145" s="40" t="s">
-        <v>479</v>
+        <v>435</v>
       </c>
       <c r="J145" s="36" t="s">
         <v>60</v>
@@ -9353,7 +9353,7 @@
         <v>191</v>
       </c>
       <c r="S145" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T145" s="36" t="s">
         <v>189</v>
@@ -9375,7 +9375,7 @@
         <v>38</v>
       </c>
       <c r="D146" s="33" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>53</v>
@@ -9387,10 +9387,10 @@
         <v>472</v>
       </c>
       <c r="H146" s="35" t="s">
-        <v>474</v>
+        <v>431</v>
       </c>
       <c r="I146" s="40" t="s">
-        <v>479</v>
+        <v>435</v>
       </c>
       <c r="J146" s="36" t="s">
         <v>60</v>
@@ -9414,7 +9414,7 @@
         <v>191</v>
       </c>
       <c r="S146" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T146" s="36" t="s">
         <v>189</v>
@@ -9436,7 +9436,7 @@
         <v>38</v>
       </c>
       <c r="D147" s="33" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="E147" s="41" t="s">
         <v>333</v>
@@ -9445,7 +9445,7 @@
         <v>46030</v>
       </c>
       <c r="G147" s="35" t="s">
-        <v>468</v>
+        <v>494</v>
       </c>
       <c r="H147" s="35"/>
       <c r="I147" s="40"/>
@@ -9471,7 +9471,7 @@
         <v>191</v>
       </c>
       <c r="S147" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T147" s="36" t="s">
         <v>189</v>
@@ -9493,7 +9493,7 @@
         <v>38</v>
       </c>
       <c r="D148" s="33" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="E148" s="41" t="s">
         <v>332</v>
@@ -9502,13 +9502,13 @@
         <v>46018</v>
       </c>
       <c r="G148" s="35" t="s">
-        <v>401</v>
+        <v>473</v>
       </c>
       <c r="H148" s="35" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="I148" s="40" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="J148" s="36" t="s">
         <v>60</v>
@@ -9542,7 +9542,7 @@
         <v>38</v>
       </c>
       <c r="D149" s="33" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>332</v>
@@ -9551,13 +9551,13 @@
         <v>46018</v>
       </c>
       <c r="G149" s="35" t="s">
-        <v>405</v>
+        <v>474</v>
       </c>
       <c r="H149" s="35" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="I149" s="40" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="J149" s="36" t="s">
         <v>60</v>
@@ -9591,7 +9591,7 @@
         <v>38</v>
       </c>
       <c r="D150" s="33" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="E150" s="41" t="s">
         <v>332</v>
@@ -9600,13 +9600,13 @@
         <v>46019</v>
       </c>
       <c r="G150" s="35" t="s">
-        <v>408</v>
+        <v>475</v>
       </c>
       <c r="H150" s="35" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="I150" s="40" t="s">
-        <v>480</v>
+        <v>436</v>
       </c>
       <c r="J150" s="36" t="s">
         <v>60</v>
@@ -9630,7 +9630,7 @@
         <v>191</v>
       </c>
       <c r="S150" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T150" s="36" t="s">
         <v>189</v>
@@ -9654,7 +9654,7 @@
         <v>38</v>
       </c>
       <c r="D151" s="33" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="E151" s="41" t="s">
         <v>332</v>
@@ -9663,13 +9663,13 @@
         <v>46019</v>
       </c>
       <c r="G151" s="35" t="s">
-        <v>410</v>
+        <v>476</v>
       </c>
       <c r="H151" s="35" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="I151" s="40" t="s">
-        <v>481</v>
+        <v>437</v>
       </c>
       <c r="J151" s="36" t="s">
         <v>60</v>
@@ -9693,7 +9693,7 @@
         <v>191</v>
       </c>
       <c r="S151" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T151" s="36" t="s">
         <v>189</v>
@@ -9717,7 +9717,7 @@
         <v>38</v>
       </c>
       <c r="D152" s="33" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>332</v>
@@ -9726,13 +9726,13 @@
         <v>46019</v>
       </c>
       <c r="G152" s="35" t="s">
-        <v>412</v>
+        <v>477</v>
       </c>
       <c r="H152" s="35" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="I152" s="40" t="s">
-        <v>482</v>
+        <v>438</v>
       </c>
       <c r="J152" s="36" t="s">
         <v>60</v>
@@ -9756,7 +9756,7 @@
         <v>191</v>
       </c>
       <c r="S152" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T152" s="36" t="s">
         <v>189</v>
@@ -9780,7 +9780,7 @@
         <v>38</v>
       </c>
       <c r="D153" s="33" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="E153" s="41" t="s">
         <v>332</v>
@@ -9789,13 +9789,13 @@
         <v>46019</v>
       </c>
       <c r="G153" s="35" t="s">
-        <v>414</v>
+        <v>478</v>
       </c>
       <c r="H153" s="35" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
       <c r="I153" s="40" t="s">
-        <v>483</v>
+        <v>439</v>
       </c>
       <c r="J153" s="36" t="s">
         <v>60</v>
@@ -9819,7 +9819,7 @@
         <v>191</v>
       </c>
       <c r="S153" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T153" s="36" t="s">
         <v>189</v>
@@ -9843,7 +9843,7 @@
         <v>38</v>
       </c>
       <c r="D154" s="33" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="E154" s="41" t="s">
         <v>332</v>
@@ -9852,13 +9852,13 @@
         <v>46019</v>
       </c>
       <c r="G154" s="35" t="s">
-        <v>416</v>
+        <v>479</v>
       </c>
       <c r="H154" s="35" t="s">
-        <v>417</v>
+        <v>390</v>
       </c>
       <c r="I154" s="40" t="s">
-        <v>484</v>
+        <v>440</v>
       </c>
       <c r="J154" s="36" t="s">
         <v>60</v>
@@ -9882,7 +9882,7 @@
         <v>191</v>
       </c>
       <c r="S154" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T154" s="36" t="s">
         <v>189</v>
@@ -9906,7 +9906,7 @@
         <v>38</v>
       </c>
       <c r="D155" s="33" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>332</v>
@@ -9915,13 +9915,13 @@
         <v>46019</v>
       </c>
       <c r="G155" s="35" t="s">
-        <v>418</v>
+        <v>480</v>
       </c>
       <c r="H155" s="35" t="s">
-        <v>419</v>
+        <v>391</v>
       </c>
       <c r="I155" s="40" t="s">
-        <v>485</v>
+        <v>441</v>
       </c>
       <c r="J155" s="36" t="s">
         <v>60</v>
@@ -9945,7 +9945,7 @@
         <v>191</v>
       </c>
       <c r="S155" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T155" s="36" t="s">
         <v>189</v>
@@ -9969,7 +9969,7 @@
         <v>38</v>
       </c>
       <c r="D156" s="33" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="E156" s="41" t="s">
         <v>332</v>
@@ -9978,13 +9978,13 @@
         <v>46019</v>
       </c>
       <c r="G156" s="35" t="s">
-        <v>420</v>
+        <v>481</v>
       </c>
       <c r="H156" s="35" t="s">
-        <v>421</v>
+        <v>392</v>
       </c>
       <c r="I156" s="40" t="s">
-        <v>486</v>
+        <v>442</v>
       </c>
       <c r="J156" s="36" t="s">
         <v>60</v>
@@ -10008,7 +10008,7 @@
         <v>191</v>
       </c>
       <c r="S156" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T156" s="36" t="s">
         <v>189</v>
@@ -10032,7 +10032,7 @@
         <v>38</v>
       </c>
       <c r="D157" s="33" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="E157" s="41" t="s">
         <v>332</v>
@@ -10041,13 +10041,13 @@
         <v>46019</v>
       </c>
       <c r="G157" s="35" t="s">
-        <v>422</v>
+        <v>482</v>
       </c>
       <c r="H157" s="35" t="s">
-        <v>423</v>
+        <v>393</v>
       </c>
       <c r="I157" s="40" t="s">
-        <v>487</v>
+        <v>443</v>
       </c>
       <c r="J157" s="36" t="s">
         <v>60</v>
@@ -10071,7 +10071,7 @@
         <v>191</v>
       </c>
       <c r="S157" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T157" s="36" t="s">
         <v>189</v>
@@ -10095,7 +10095,7 @@
         <v>38</v>
       </c>
       <c r="D158" s="33" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>332</v>
@@ -10104,13 +10104,13 @@
         <v>46019</v>
       </c>
       <c r="G158" s="35" t="s">
-        <v>424</v>
+        <v>483</v>
       </c>
       <c r="H158" s="35" t="s">
-        <v>425</v>
+        <v>394</v>
       </c>
       <c r="I158" s="40" t="s">
-        <v>488</v>
+        <v>444</v>
       </c>
       <c r="J158" s="36" t="s">
         <v>60</v>
@@ -10134,7 +10134,7 @@
         <v>191</v>
       </c>
       <c r="S158" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T158" s="36" t="s">
         <v>189</v>
@@ -10158,7 +10158,7 @@
         <v>38</v>
       </c>
       <c r="D159" s="33" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="E159" s="41" t="s">
         <v>332</v>
@@ -10167,13 +10167,13 @@
         <v>46019</v>
       </c>
       <c r="G159" s="35" t="s">
-        <v>426</v>
+        <v>484</v>
       </c>
       <c r="H159" s="35" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="I159" s="40" t="s">
-        <v>489</v>
+        <v>445</v>
       </c>
       <c r="J159" s="36" t="s">
         <v>60</v>
@@ -10197,7 +10197,7 @@
         <v>191</v>
       </c>
       <c r="S159" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T159" s="36" t="s">
         <v>189</v>
@@ -10221,7 +10221,7 @@
         <v>38</v>
       </c>
       <c r="D160" s="33" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="E160" s="41" t="s">
         <v>332</v>
@@ -10230,13 +10230,13 @@
         <v>46019</v>
       </c>
       <c r="G160" s="35" t="s">
-        <v>428</v>
+        <v>485</v>
       </c>
       <c r="H160" s="35" t="s">
-        <v>429</v>
+        <v>396</v>
       </c>
       <c r="I160" s="40" t="s">
-        <v>490</v>
+        <v>446</v>
       </c>
       <c r="J160" s="36" t="s">
         <v>60</v>
@@ -10260,7 +10260,7 @@
         <v>191</v>
       </c>
       <c r="S160" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T160" s="36" t="s">
         <v>189</v>
@@ -10284,7 +10284,7 @@
         <v>38</v>
       </c>
       <c r="D161" s="33" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>332</v>
@@ -10293,13 +10293,13 @@
         <v>46019</v>
       </c>
       <c r="G161" s="35" t="s">
-        <v>430</v>
+        <v>486</v>
       </c>
       <c r="H161" s="35" t="s">
-        <v>431</v>
+        <v>397</v>
       </c>
       <c r="I161" s="40" t="s">
-        <v>491</v>
+        <v>447</v>
       </c>
       <c r="J161" s="36" t="s">
         <v>60</v>
@@ -10323,7 +10323,7 @@
         <v>191</v>
       </c>
       <c r="S161" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T161" s="36" t="s">
         <v>189</v>
@@ -10347,7 +10347,7 @@
         <v>38</v>
       </c>
       <c r="D162" s="33" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="E162" s="41" t="s">
         <v>332</v>
@@ -10356,13 +10356,13 @@
         <v>46019</v>
       </c>
       <c r="G162" s="35" t="s">
-        <v>432</v>
+        <v>487</v>
       </c>
       <c r="H162" s="35" t="s">
-        <v>433</v>
+        <v>398</v>
       </c>
       <c r="I162" s="40" t="s">
-        <v>492</v>
+        <v>448</v>
       </c>
       <c r="J162" s="36" t="s">
         <v>60</v>
@@ -10386,7 +10386,7 @@
         <v>191</v>
       </c>
       <c r="S162" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T162" s="36" t="s">
         <v>189</v>
@@ -10410,7 +10410,7 @@
         <v>38</v>
       </c>
       <c r="D163" s="33" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="E163" s="41" t="s">
         <v>332</v>
@@ -10419,13 +10419,13 @@
         <v>46019</v>
       </c>
       <c r="G163" s="35" t="s">
-        <v>434</v>
+        <v>488</v>
       </c>
       <c r="H163" s="35" t="s">
-        <v>435</v>
+        <v>399</v>
       </c>
       <c r="I163" s="40" t="s">
-        <v>493</v>
+        <v>449</v>
       </c>
       <c r="J163" s="36" t="s">
         <v>60</v>
@@ -10449,7 +10449,7 @@
         <v>191</v>
       </c>
       <c r="S163" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T163" s="36" t="s">
         <v>189</v>
@@ -10473,7 +10473,7 @@
         <v>38</v>
       </c>
       <c r="D164" s="33" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>332</v>
@@ -10482,13 +10482,13 @@
         <v>46019</v>
       </c>
       <c r="G164" s="35" t="s">
-        <v>436</v>
+        <v>489</v>
       </c>
       <c r="H164" s="35" t="s">
-        <v>437</v>
+        <v>400</v>
       </c>
       <c r="I164" s="40" t="s">
-        <v>494</v>
+        <v>450</v>
       </c>
       <c r="J164" s="36" t="s">
         <v>60</v>
@@ -10512,7 +10512,7 @@
         <v>191</v>
       </c>
       <c r="S164" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T164" s="36" t="s">
         <v>189</v>
@@ -10536,7 +10536,7 @@
         <v>38</v>
       </c>
       <c r="D165" s="33" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
       <c r="E165" s="41" t="s">
         <v>332</v>
@@ -10545,13 +10545,13 @@
         <v>46019</v>
       </c>
       <c r="G165" s="35" t="s">
-        <v>438</v>
+        <v>490</v>
       </c>
       <c r="H165" s="35" t="s">
-        <v>439</v>
+        <v>401</v>
       </c>
       <c r="I165" s="40" t="s">
-        <v>495</v>
+        <v>451</v>
       </c>
       <c r="J165" s="36" t="s">
         <v>60</v>
@@ -10575,7 +10575,7 @@
         <v>191</v>
       </c>
       <c r="S165" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T165" s="36" t="s">
         <v>189</v>
@@ -10599,7 +10599,7 @@
         <v>38</v>
       </c>
       <c r="D166" s="33" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="E166" s="41" t="s">
         <v>332</v>
@@ -10608,13 +10608,13 @@
         <v>46019</v>
       </c>
       <c r="G166" s="35" t="s">
-        <v>440</v>
+        <v>491</v>
       </c>
       <c r="H166" s="35" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="I166" s="40" t="s">
-        <v>496</v>
+        <v>452</v>
       </c>
       <c r="J166" s="36" t="s">
         <v>60</v>
@@ -10638,7 +10638,7 @@
         <v>191</v>
       </c>
       <c r="S166" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T166" s="36" t="s">
         <v>189</v>
@@ -10662,7 +10662,7 @@
         <v>38</v>
       </c>
       <c r="D167" s="33" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>332</v>
@@ -10671,13 +10671,13 @@
         <v>46019</v>
       </c>
       <c r="G167" s="35" t="s">
-        <v>442</v>
+        <v>492</v>
       </c>
       <c r="H167" s="35" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="I167" s="40" t="s">
-        <v>497</v>
+        <v>453</v>
       </c>
       <c r="J167" s="36" t="s">
         <v>60</v>
@@ -10701,7 +10701,7 @@
         <v>191</v>
       </c>
       <c r="S167" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T167" s="36" t="s">
         <v>189</v>
@@ -10725,7 +10725,7 @@
         <v>48</v>
       </c>
       <c r="D168" s="33" t="s">
-        <v>466</v>
+        <v>426</v>
       </c>
       <c r="E168" s="41" t="s">
         <v>43</v>
@@ -10734,13 +10734,13 @@
         <v>46031</v>
       </c>
       <c r="G168" s="35" t="s">
-        <v>476</v>
+        <v>493</v>
       </c>
       <c r="H168" s="35" t="s">
-        <v>475</v>
+        <v>432</v>
       </c>
       <c r="I168" s="40" t="s">
-        <v>479</v>
+        <v>435</v>
       </c>
       <c r="J168" s="36" t="s">
         <v>60</v>
@@ -10764,7 +10764,7 @@
         <v>191</v>
       </c>
       <c r="S168" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T168" s="36" t="s">
         <v>189</v>
@@ -10786,7 +10786,7 @@
         <v>48</v>
       </c>
       <c r="D169" s="33" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="E169" s="41" t="s">
         <v>53</v>
@@ -10795,13 +10795,13 @@
         <v>46031</v>
       </c>
       <c r="G169" s="35" t="s">
-        <v>476</v>
+        <v>493</v>
       </c>
       <c r="H169" s="35" t="s">
-        <v>477</v>
+        <v>433</v>
       </c>
       <c r="I169" s="40" t="s">
-        <v>479</v>
+        <v>435</v>
       </c>
       <c r="J169" s="36" t="s">
         <v>60</v>
@@ -10825,7 +10825,7 @@
         <v>191</v>
       </c>
       <c r="S169" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T169" s="36" t="s">
         <v>189</v>
@@ -10847,7 +10847,7 @@
         <v>48</v>
       </c>
       <c r="D170" s="33" t="s">
-        <v>463</v>
+        <v>423</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>333</v>
@@ -10856,7 +10856,7 @@
         <v>46030</v>
       </c>
       <c r="G170" s="35" t="s">
-        <v>469</v>
+        <v>495</v>
       </c>
       <c r="H170" s="35"/>
       <c r="I170" s="40"/>
@@ -10882,7 +10882,7 @@
         <v>191</v>
       </c>
       <c r="S170" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T170" s="36" t="s">
         <v>189</v>
@@ -10913,7 +10913,7 @@
         <v>46017</v>
       </c>
       <c r="G171" s="35" t="s">
-        <v>360</v>
+        <v>496</v>
       </c>
       <c r="H171" s="35" t="s">
         <v>352</v>
@@ -11073,7 +11073,7 @@
         <v>46017</v>
       </c>
       <c r="G175" s="35" t="s">
-        <v>361</v>
+        <v>497</v>
       </c>
       <c r="H175" s="35" t="s">
         <v>354</v>
@@ -11122,13 +11122,13 @@
         <v>46018</v>
       </c>
       <c r="G176" s="35" t="s">
-        <v>359</v>
+        <v>498</v>
       </c>
       <c r="H176" s="35" t="s">
         <v>358</v>
       </c>
       <c r="I176" s="40" t="s">
-        <v>498</v>
+        <v>454</v>
       </c>
       <c r="J176" s="36" t="s">
         <v>60</v>
@@ -11152,7 +11152,7 @@
         <v>191</v>
       </c>
       <c r="S176" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T176" s="36" t="s">
         <v>189</v>
@@ -11176,7 +11176,7 @@
         <v>48</v>
       </c>
       <c r="D177" s="33" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E177" s="41" t="s">
         <v>332</v>
@@ -11185,13 +11185,13 @@
         <v>46018</v>
       </c>
       <c r="G177" s="35" t="s">
-        <v>364</v>
+        <v>499</v>
       </c>
       <c r="H177" s="35" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I177" s="40" t="s">
-        <v>499</v>
+        <v>455</v>
       </c>
       <c r="J177" s="36" t="s">
         <v>60</v>
@@ -11215,7 +11215,7 @@
         <v>191</v>
       </c>
       <c r="S177" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T177" s="36" t="s">
         <v>189</v>
@@ -11239,7 +11239,7 @@
         <v>48</v>
       </c>
       <c r="D178" s="33" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E178" s="41" t="s">
         <v>332</v>
@@ -11248,13 +11248,13 @@
         <v>46018</v>
       </c>
       <c r="G178" s="35" t="s">
-        <v>366</v>
+        <v>500</v>
       </c>
       <c r="H178" s="35" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="I178" s="40" t="s">
-        <v>500</v>
+        <v>456</v>
       </c>
       <c r="J178" s="36" t="s">
         <v>60</v>
@@ -11278,7 +11278,7 @@
         <v>191</v>
       </c>
       <c r="S178" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T178" s="36" t="s">
         <v>189</v>
@@ -11311,13 +11311,13 @@
         <v>46018</v>
       </c>
       <c r="G179" s="35" t="s">
-        <v>368</v>
+        <v>501</v>
       </c>
       <c r="H179" s="35" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="I179" s="40" t="s">
-        <v>501</v>
+        <v>457</v>
       </c>
       <c r="J179" s="36" t="s">
         <v>60</v>
@@ -11341,7 +11341,7 @@
         <v>191</v>
       </c>
       <c r="S179" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T179" s="36" t="s">
         <v>189</v>
@@ -11374,13 +11374,13 @@
         <v>46018</v>
       </c>
       <c r="G180" s="35" t="s">
-        <v>370</v>
+        <v>502</v>
       </c>
       <c r="H180" s="35" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="I180" s="40" t="s">
-        <v>502</v>
+        <v>458</v>
       </c>
       <c r="J180" s="36" t="s">
         <v>60</v>
@@ -11404,7 +11404,7 @@
         <v>191</v>
       </c>
       <c r="S180" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T180" s="36" t="s">
         <v>189</v>
@@ -11437,13 +11437,13 @@
         <v>46018</v>
       </c>
       <c r="G181" s="35" t="s">
-        <v>372</v>
+        <v>503</v>
       </c>
       <c r="H181" s="35" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I181" s="40" t="s">
-        <v>503</v>
+        <v>459</v>
       </c>
       <c r="J181" s="36" t="s">
         <v>60</v>
@@ -11467,7 +11467,7 @@
         <v>191</v>
       </c>
       <c r="S181" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T181" s="36" t="s">
         <v>189</v>
@@ -11500,13 +11500,13 @@
         <v>46018</v>
       </c>
       <c r="G182" s="35" t="s">
-        <v>374</v>
+        <v>504</v>
       </c>
       <c r="H182" s="35" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="I182" s="40" t="s">
-        <v>504</v>
+        <v>460</v>
       </c>
       <c r="J182" s="36" t="s">
         <v>60</v>
@@ -11530,7 +11530,7 @@
         <v>191</v>
       </c>
       <c r="S182" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T182" s="36" t="s">
         <v>189</v>
@@ -11563,13 +11563,13 @@
         <v>46018</v>
       </c>
       <c r="G183" s="35" t="s">
-        <v>376</v>
+        <v>505</v>
       </c>
       <c r="H183" s="35" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="I183" s="40" t="s">
-        <v>505</v>
+        <v>461</v>
       </c>
       <c r="J183" s="36" t="s">
         <v>60</v>
@@ -11593,7 +11593,7 @@
         <v>191</v>
       </c>
       <c r="S183" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T183" s="36" t="s">
         <v>189</v>
@@ -11626,13 +11626,13 @@
         <v>46018</v>
       </c>
       <c r="G184" s="35" t="s">
-        <v>378</v>
+        <v>506</v>
       </c>
       <c r="H184" s="35" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="I184" s="40" t="s">
-        <v>506</v>
+        <v>462</v>
       </c>
       <c r="J184" s="36" t="s">
         <v>60</v>
@@ -11656,7 +11656,7 @@
         <v>191</v>
       </c>
       <c r="S184" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T184" s="36" t="s">
         <v>189</v>
@@ -11689,13 +11689,13 @@
         <v>46018</v>
       </c>
       <c r="G185" s="35" t="s">
-        <v>380</v>
+        <v>507</v>
       </c>
       <c r="H185" s="35" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="I185" s="40" t="s">
-        <v>507</v>
+        <v>463</v>
       </c>
       <c r="J185" s="36" t="s">
         <v>60</v>
@@ -11719,7 +11719,7 @@
         <v>191</v>
       </c>
       <c r="S185" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T185" s="36" t="s">
         <v>189</v>
@@ -11752,13 +11752,13 @@
         <v>46018</v>
       </c>
       <c r="G186" s="35" t="s">
-        <v>382</v>
+        <v>508</v>
       </c>
       <c r="H186" s="35" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="I186" s="40" t="s">
-        <v>508</v>
+        <v>464</v>
       </c>
       <c r="J186" s="36" t="s">
         <v>60</v>
@@ -11782,7 +11782,7 @@
         <v>191</v>
       </c>
       <c r="S186" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T186" s="36" t="s">
         <v>189</v>
@@ -11815,13 +11815,13 @@
         <v>46018</v>
       </c>
       <c r="G187" s="35" t="s">
-        <v>384</v>
+        <v>509</v>
       </c>
       <c r="H187" s="35" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="I187" s="40" t="s">
-        <v>509</v>
+        <v>465</v>
       </c>
       <c r="J187" s="36" t="s">
         <v>60</v>
@@ -11845,7 +11845,7 @@
         <v>191</v>
       </c>
       <c r="S187" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T187" s="36" t="s">
         <v>189</v>
@@ -11878,13 +11878,13 @@
         <v>46018</v>
       </c>
       <c r="G188" s="35" t="s">
-        <v>386</v>
+        <v>510</v>
       </c>
       <c r="H188" s="35" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="I188" s="40" t="s">
-        <v>510</v>
+        <v>466</v>
       </c>
       <c r="J188" s="36" t="s">
         <v>60</v>
@@ -11908,7 +11908,7 @@
         <v>191</v>
       </c>
       <c r="S188" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T188" s="36" t="s">
         <v>189</v>
@@ -11941,13 +11941,13 @@
         <v>46018</v>
       </c>
       <c r="G189" s="35" t="s">
-        <v>388</v>
+        <v>511</v>
       </c>
       <c r="H189" s="35" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="I189" s="40" t="s">
-        <v>511</v>
+        <v>467</v>
       </c>
       <c r="J189" s="36" t="s">
         <v>60</v>
@@ -11971,7 +11971,7 @@
         <v>191</v>
       </c>
       <c r="S189" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T189" s="36" t="s">
         <v>189</v>
@@ -12004,13 +12004,13 @@
         <v>46018</v>
       </c>
       <c r="G190" s="35" t="s">
-        <v>390</v>
+        <v>512</v>
       </c>
       <c r="H190" s="35" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="I190" s="40" t="s">
-        <v>512</v>
+        <v>468</v>
       </c>
       <c r="J190" s="36" t="s">
         <v>60</v>
@@ -12034,7 +12034,7 @@
         <v>191</v>
       </c>
       <c r="S190" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T190" s="36" t="s">
         <v>189</v>
@@ -12067,13 +12067,13 @@
         <v>46018</v>
       </c>
       <c r="G191" s="35" t="s">
-        <v>392</v>
+        <v>513</v>
       </c>
       <c r="H191" s="35" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="I191" s="40" t="s">
-        <v>513</v>
+        <v>469</v>
       </c>
       <c r="J191" s="36" t="s">
         <v>60</v>
@@ -12097,7 +12097,7 @@
         <v>191</v>
       </c>
       <c r="S191" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T191" s="36" t="s">
         <v>189</v>
@@ -12121,7 +12121,7 @@
         <v>48</v>
       </c>
       <c r="D192" s="33" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="E192" s="41" t="s">
         <v>332</v>
@@ -12130,13 +12130,13 @@
         <v>46018</v>
       </c>
       <c r="G192" s="35" t="s">
-        <v>395</v>
+        <v>514</v>
       </c>
       <c r="H192" s="35" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="I192" s="40" t="s">
-        <v>514</v>
+        <v>470</v>
       </c>
       <c r="J192" s="36" t="s">
         <v>60</v>
@@ -12160,7 +12160,7 @@
         <v>191</v>
       </c>
       <c r="S192" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T192" s="36" t="s">
         <v>189</v>
@@ -12184,7 +12184,7 @@
         <v>48</v>
       </c>
       <c r="D193" s="33" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="E193" s="41" t="s">
         <v>332</v>
@@ -12193,13 +12193,13 @@
         <v>46018</v>
       </c>
       <c r="G193" s="35" t="s">
-        <v>397</v>
+        <v>515</v>
       </c>
       <c r="H193" s="35" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="I193" s="40" t="s">
-        <v>515</v>
+        <v>471</v>
       </c>
       <c r="J193" s="36" t="s">
         <v>60</v>
@@ -12223,7 +12223,7 @@
         <v>191</v>
       </c>
       <c r="S193" s="36" t="s">
-        <v>478</v>
+        <v>434</v>
       </c>
       <c r="T193" s="36" t="s">
         <v>189</v>
@@ -15967,7 +15967,7 @@
         <v>471.47199999999998</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>470</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
@@ -15981,7 +15981,7 @@
         <v>448.44900000000001</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>471</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -17992,21 +17992,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -18150,31 +18135,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="295b7897-c886-40bf-9750-5782b814c3e4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18190,4 +18166,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="295b7897-c886-40bf-9750-5782b814c3e4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>